<commit_message>
Add full fucntion import and export Data, wait test
</commit_message>
<xml_diff>
--- a/YC5_API_IO/YC5_API_IO/SampleTasks.xlsx
+++ b/YC5_API_IO/YC5_API_IO/SampleTasks.xlsx
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>TaskName</t>
   </si>
   <si>
-    <t>CategoryId</t>
-  </si>
-  <si>
-    <t>UserId</t>
-  </si>
-  <si>
     <t>TaskDescription</t>
   </si>
   <si>
@@ -150,37 +144,16 @@
     <t>Bug</t>
   </si>
   <si>
-    <t>69302244-d387-4ada-89cc-420835213bd9</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd10</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd11</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd12</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd13</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd14</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd15</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd16</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd17</t>
-  </si>
-  <si>
-    <t>69302244-d387-4ada-89cc-420835213bd18</t>
-  </si>
-  <si>
-    <t>8720581f-e9fb-49d5-9fe7-5053b7c6c4ea</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Thực tập</t>
+  </si>
+  <si>
+    <t>Nguyendinhnam28803</t>
   </si>
 </sst>
 </file>
@@ -999,7 +972,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1013,288 +986,288 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>46096</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <v>46111</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>46101</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
       </c>
       <c r="G5" s="1">
         <v>46081</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1">
         <v>46122</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1">
         <v>46086</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
         <v>46084</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1">
         <v>46091</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" s="1">
         <v>46106</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1">
         <v>46099</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>